<commit_message>
SAC identifiers version 2308
Update Semi-Annual Enterprise Channel identifiers for version 2308 (Build 16731.20504)
</commit_message>
<xml_diff>
--- a/Microsoft 365/Semi-Annual Enterprise Channel/outlookmmseditcontrols.xlsx
+++ b/Microsoft 365/Semi-Annual Enterprise Channel/outlookmmseditcontrols.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26410"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27315"/>
+  <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bcoard\OneDrive - Microsoft\Documents\RibbonX Upload\SAC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TcidDocs\SACJuly2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3D80126A-F25C-4EFD-BA6F-EA0B026BD406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C5424654-325C-4696-B836-A8B483F70D2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="43200" windowHeight="23325"/>
+    <workbookView xWindow="0" yWindow="5415" windowWidth="51600" windowHeight="15465"/>
   </bookViews>
   <sheets>
     <sheet name="outlookmmseditcontrols" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="146">
   <si>
     <t>Policy ID</t>
   </si>
@@ -452,6 +452,9 @@
   </si>
   <si>
     <t>OutlookFeedbackUIF</t>
+  </si>
+  <si>
+    <t>OfficeFeedbackBackstage</t>
   </si>
   <si>
     <t>Column1</t>
@@ -465,21 +468,21 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Calibri Light"/>
+      <name val="Aptos Display"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
@@ -487,7 +490,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -495,7 +498,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -503,35 +506,35 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -539,7 +542,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -547,14 +550,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -562,14 +565,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -577,7 +580,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -585,14 +588,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -646,19 +649,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.7999816888943144"/>
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.5999938962981048"/>
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.3999755851924192"/>
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -669,19 +672,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.7999816888943144"/>
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.5999938962981048"/>
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.3999755851924192"/>
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -692,19 +695,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.7999816888943144"/>
+        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.5999938962981048"/>
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.3999755851924192"/>
+        <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -715,19 +718,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.7999816888943144"/>
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.5999938962981048"/>
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.3999755851924192"/>
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -738,19 +741,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.7999816888943144"/>
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.5999938962981048"/>
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.3999755851924192"/>
+        <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -761,19 +764,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.7999816888943144"/>
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.5999938962981048"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.3999755851924192"/>
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -809,7 +812,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.3999755851924192"/>
+        <color theme="4" tint="0.39997558519241921"/>
       </bottom>
       <diagonal/>
     </border>
@@ -999,8 +1002,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I152" totalsRowShown="0">
-  <autoFilter ref="A1:I152"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I153" totalsRowShown="0">
+  <autoFilter ref="A1:I153"/>
   <tableColumns count="9">
     <tableColumn id="1" name="Control Name"/>
     <tableColumn id="2" name="Control Type"/>
@@ -1027,39 +1030,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="0E2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="E8E8E8"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="156082"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="E97132"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="196B24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="0F9ED5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="A02B93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1111,7 +1114,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1222,13 +1225,6 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -1237,6 +1233,13 @@
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1301,11 +1304,31 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1313,7 +1336,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I152"/>
+  <dimension ref="A1:I153"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:A1048576"/>
@@ -1321,15 +1344,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.5703125" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" customWidth="1"/>
-    <col min="9" max="9" width="11" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.140625" customWidth="1"/>
+    <col min="8" max="8" width="11" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -1358,7 +1381,7 @@
         <v>0</v>
       </c>
       <c r="I1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -3952,15 +3975,29 @@
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
+        <v>144</v>
+      </c>
+      <c r="B152" t="s">
+        <v>9</v>
+      </c>
+      <c r="C152" t="s">
+        <v>93</v>
+      </c>
+      <c r="H152">
+        <v>27302</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
         <v>60</v>
       </c>
-      <c r="B152" t="s">
-        <v>9</v>
-      </c>
-      <c r="C152" t="s">
-        <v>93</v>
-      </c>
-      <c r="H152">
+      <c r="B153" t="s">
+        <v>9</v>
+      </c>
+      <c r="C153" t="s">
+        <v>93</v>
+      </c>
+      <c r="H153">
         <v>11323</v>
       </c>
     </row>

</xml_diff>